<commit_message>
EPBDS-7343 DT tables doesn't work with formulas
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7343_DT_with_formulas.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7343_DT_with_formulas.xlsx
@@ -4,10 +4,11 @@
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="DT" sheetId="13" r:id="rId1"/>
+    <sheet name="Tests" sheetId="14" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_st1">#REF!</definedName>
@@ -19,8 +20,33 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Автор</author>
+  </authors>
+  <commentList>
+    <comment ref="B26" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+            <charset val="204"/>
+          </rPr>
+          <t xml:space="preserve">OpenL Tablets automatically recognizes condition expression as  "min &lt;= hour  and  hour &lt; max".
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
   <si>
     <t>Value</t>
   </si>
@@ -76,17 +102,71 @@
     <t>0</t>
   </si>
   <si>
-    <t>SimpleRules Double dt2(Double val)</t>
-  </si>
-  <si>
     <t>9,8,7</t>
+  </si>
+  <si>
+    <t>Rules Double dt2(Double val)</t>
+  </si>
+  <si>
+    <t>SimpleRules Double dt4(Double val)</t>
+  </si>
+  <si>
+    <t>SimpleRules Double dt3(Double val)</t>
+  </si>
+  <si>
+    <t>Test dt1 dt1_Test</t>
+  </si>
+  <si>
+    <t>Test dt4 dt4_Test</t>
+  </si>
+  <si>
+    <t>Test dt3 dt3_Test</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>Integer min</t>
+  </si>
+  <si>
+    <t>Integer max</t>
+  </si>
+  <si>
+    <t>From</t>
+  </si>
+  <si>
+    <t>To</t>
+  </si>
+  <si>
+    <t>Integer ret</t>
+  </si>
+  <si>
+    <r>
+      <t>Rules String dt5</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="0" tint="-0.499984740745262"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="204"/>
+      </rPr>
+      <t xml:space="preserve"> (Integer hour)</t>
+    </r>
+  </si>
+  <si>
+    <t>Test dt5 dt5_Test</t>
+  </si>
+  <si>
+    <t>Hour</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="7">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -102,34 +182,63 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000001"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="11"/>
       <color indexed="8"/>
-      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000001"/>
-      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -162,8 +271,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF6DB66"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -186,32 +319,101 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
@@ -553,215 +755,919 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B4:C33"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:L40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B40" sqref="B40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="41.28515625" customWidth="1" collapsed="1"/>
     <col min="3" max="3" width="55.140625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="19.28515625" customWidth="1"/>
+    <col min="6" max="6" width="42" customWidth="1"/>
+    <col min="7" max="7" width="65.42578125" customWidth="1"/>
+    <col min="8" max="8" width="31.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="2:3">
-      <c r="B4" s="7" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="2"/>
+      <c r="G2" s="2"/>
+      <c r="H2" s="2"/>
+      <c r="I2" s="2"/>
+      <c r="J2" s="2"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
+      <c r="G3" s="2"/>
+      <c r="H3" s="2"/>
+      <c r="I3" s="2"/>
+      <c r="J3" s="2"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2"/>
+      <c r="B4" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="15" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="2:3">
-      <c r="B5" s="2" t="s">
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="15" t="s">
+        <v>19</v>
+      </c>
+      <c r="G4" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="2"/>
+      <c r="K4" s="3"/>
+      <c r="L4" s="3"/>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="4" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="2:3">
-      <c r="B6" s="2" t="s">
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="2"/>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2"/>
+      <c r="B6" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="4" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="2:3">
-      <c r="B7" s="2"/>
-      <c r="C7" s="2" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="2"/>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3"/>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="8" spans="2:3">
-      <c r="B8" s="3" t="s">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="2"/>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3"/>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2"/>
+      <c r="B8" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="6" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="2:3">
-      <c r="B9" s="5" t="s">
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="2"/>
+      <c r="K8" s="3"/>
+      <c r="L8" s="3"/>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2"/>
+      <c r="B9" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="2:3">
-      <c r="B10" s="5" t="s">
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="8">
+        <v>1</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="2"/>
+      <c r="K9" s="3"/>
+      <c r="L9" s="3"/>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="8">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="2:3">
-      <c r="B11" s="5">
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G10" s="8">
+        <v>2</v>
+      </c>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="2"/>
+      <c r="K10" s="3"/>
+      <c r="L10" s="3"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2"/>
+      <c r="B11" s="7">
         <v>3</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="8" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="12" spans="2:3">
-      <c r="B12" s="5" t="s">
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="7">
+        <v>3</v>
+      </c>
+      <c r="G11" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="2"/>
+      <c r="K11" s="3"/>
+      <c r="L11" s="3"/>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2"/>
+      <c r="B12" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="8">
         <v>3</v>
       </c>
-    </row>
-    <row r="13" spans="2:3">
-      <c r="B13" s="5">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="7">
+        <v>4</v>
+      </c>
+      <c r="G12" s="8">
+        <v>3</v>
+      </c>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="2"/>
+      <c r="K12" s="3"/>
+      <c r="L12" s="3"/>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="2"/>
+      <c r="B13" s="7">
         <v>5</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="8">
         <v>4</v>
       </c>
-    </row>
-    <row r="16" spans="2:3">
-      <c r="B16" s="7" t="s">
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="7">
+        <v>5</v>
+      </c>
+      <c r="G13" s="8">
+        <v>4</v>
+      </c>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="2"/>
+      <c r="K13" s="3"/>
+      <c r="L13" s="3"/>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="2"/>
+      <c r="K14" s="3"/>
+      <c r="L14" s="3"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="2"/>
+      <c r="K15" s="3"/>
+      <c r="L15" s="3"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="2"/>
+      <c r="B16" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="G16" s="15" t="s">
+        <v>7</v>
+      </c>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="2"/>
+      <c r="K16" s="3"/>
+      <c r="L16" s="3"/>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2"/>
+      <c r="B17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G17" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="2"/>
+      <c r="K17" s="3"/>
+      <c r="L17" s="3"/>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2"/>
+      <c r="B18" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="C16" s="7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="17" spans="2:3">
-      <c r="B17" s="3" t="s">
+      <c r="C18" s="8">
+        <v>1</v>
+      </c>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="G18" s="8">
+        <v>1</v>
+      </c>
+      <c r="H18" s="2"/>
+      <c r="I18" s="2"/>
+      <c r="J18" s="2"/>
+      <c r="K18" s="3"/>
+      <c r="L18" s="3"/>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2"/>
+      <c r="B19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="C19" s="8">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="G19" s="8">
+        <v>2</v>
+      </c>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="2"/>
+      <c r="K19" s="3"/>
+      <c r="L19" s="3"/>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2"/>
+      <c r="B20" s="7">
+        <v>3</v>
+      </c>
+      <c r="C20" s="8">
         <v>0</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="7">
+        <v>3</v>
+      </c>
+      <c r="G20" s="8">
+        <v>0</v>
+      </c>
+      <c r="H20" s="2"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="2"/>
+      <c r="K20" s="3"/>
+      <c r="L20" s="3"/>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2"/>
+      <c r="B21" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C21" s="8">
+        <v>3</v>
+      </c>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="7">
+        <v>4</v>
+      </c>
+      <c r="G21" s="8">
+        <v>3</v>
+      </c>
+      <c r="H21" s="2"/>
+      <c r="I21" s="2"/>
+      <c r="J21" s="2"/>
+      <c r="K21" s="3"/>
+      <c r="L21" s="3"/>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
+      <c r="H22" s="2"/>
+      <c r="I22" s="2"/>
+      <c r="J22" s="2"/>
+      <c r="K22" s="3"/>
+      <c r="L22" s="3"/>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
+      <c r="H23" s="2"/>
+      <c r="I23" s="2"/>
+      <c r="J23" s="2"/>
+      <c r="K23" s="3"/>
+      <c r="L23" s="3"/>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A24" s="2"/>
+      <c r="B24" s="16" t="s">
+        <v>31</v>
+      </c>
+      <c r="C24" s="17"/>
+      <c r="D24" s="18"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
+      <c r="H24" s="3"/>
+      <c r="I24" s="2"/>
+      <c r="J24" s="2"/>
+      <c r="K24" s="3"/>
+      <c r="L24" s="3"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A25" s="2"/>
+      <c r="B25" s="19" t="s">
+        <v>2</v>
+      </c>
+      <c r="C25" s="19"/>
+      <c r="D25" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="E25" s="2"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="2"/>
+      <c r="K25" s="3"/>
+      <c r="L25" s="3"/>
+    </row>
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A26" s="2"/>
+      <c r="B26" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="C26" s="19"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
+      <c r="H26" s="2"/>
+      <c r="I26" s="2"/>
+      <c r="J26" s="3"/>
+      <c r="K26" s="3"/>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="2"/>
+      <c r="B27" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="C27" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E27" s="2"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="2"/>
+      <c r="K27" s="3"/>
+      <c r="L27" s="3"/>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="2"/>
+      <c r="B28" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C28" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D28" s="11" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="18" spans="2:3">
-      <c r="B18" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C18" s="6">
+      <c r="E28" s="2"/>
+      <c r="F28" s="3"/>
+      <c r="G28" s="3"/>
+      <c r="H28" s="3"/>
+      <c r="I28" s="2"/>
+      <c r="J28" s="2"/>
+      <c r="K28" s="3"/>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="B29" s="12">
+        <v>0</v>
+      </c>
+      <c r="C29" s="12">
+        <v>12</v>
+      </c>
+      <c r="D29" s="13">
         <v>1</v>
       </c>
-    </row>
-    <row r="19" spans="2:3">
-      <c r="B19" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C19" s="6">
+      <c r="E29" s="2"/>
+      <c r="F29" s="3"/>
+      <c r="G29" s="3"/>
+      <c r="H29" s="3"/>
+      <c r="I29" s="2"/>
+      <c r="J29" s="2"/>
+      <c r="K29" s="3"/>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="2"/>
+      <c r="B30" s="12">
+        <v>12</v>
+      </c>
+      <c r="C30" s="12">
+        <v>18</v>
+      </c>
+      <c r="D30" s="13">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="2:3">
-      <c r="B20" s="5">
+      <c r="E30" s="2"/>
+      <c r="F30" s="3"/>
+      <c r="G30" s="3"/>
+      <c r="H30" s="3"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="3"/>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="2"/>
+      <c r="B31" s="12">
+        <v>18</v>
+      </c>
+      <c r="C31" s="12">
+        <v>22</v>
+      </c>
+      <c r="D31" s="13">
         <v>3</v>
       </c>
-      <c r="C20" s="6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="2:3">
-      <c r="B21" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C21" s="6">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="24" spans="2:3">
-      <c r="B24" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="25" spans="2:3">
-      <c r="B25" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="26" spans="2:3">
-      <c r="B26" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="2:3">
-      <c r="B27" s="1">
+      <c r="E31" s="2"/>
+      <c r="F31" s="3"/>
+      <c r="G31" s="3"/>
+      <c r="H31" s="3"/>
+      <c r="I31" s="2"/>
+      <c r="J31" s="2"/>
+      <c r="K31" s="3"/>
+      <c r="L31" s="3"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="2"/>
+      <c r="B32" s="14">
+        <v>22</v>
+      </c>
+      <c r="C32" s="14">
+        <v>24</v>
+      </c>
+      <c r="D32" s="13">
         <v>4</v>
       </c>
-      <c r="C27" s="1">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="30" spans="2:3">
-      <c r="B30" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="C30" s="8" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="31" spans="2:3">
-      <c r="B31" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="32" spans="2:3">
-      <c r="B32" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="2:3">
-      <c r="B33" s="1">
-        <v>9</v>
-      </c>
-      <c r="C33" s="1">
-        <v>1</v>
-      </c>
+      <c r="E32" s="2"/>
+      <c r="F32" s="3"/>
+      <c r="G32" s="3"/>
+      <c r="H32" s="3"/>
+      <c r="I32" s="2"/>
+      <c r="J32" s="2"/>
+      <c r="K32" s="3"/>
+      <c r="L32" s="3"/>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="3"/>
+      <c r="G33" s="3"/>
+      <c r="H33" s="3"/>
+      <c r="I33" s="2"/>
+      <c r="J33" s="2"/>
+      <c r="K33" s="3"/>
+      <c r="L33" s="3"/>
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
+      <c r="H34" s="2"/>
+      <c r="I34" s="2"/>
+      <c r="J34" s="2"/>
+      <c r="K34" s="3"/>
+      <c r="L34" s="3"/>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2"/>
+      <c r="I35" s="2"/>
+      <c r="J35" s="2"/>
+      <c r="K35" s="3"/>
+      <c r="L35" s="3"/>
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2"/>
+      <c r="I36" s="2"/>
+      <c r="J36" s="2"/>
+      <c r="K36" s="3"/>
+      <c r="L36" s="3"/>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
+      <c r="H37" s="2"/>
+      <c r="I37" s="2"/>
+      <c r="J37" s="2"/>
+      <c r="K37" s="3"/>
+      <c r="L37" s="3"/>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
+      <c r="H38" s="2"/>
+      <c r="I38" s="2"/>
+      <c r="J38" s="2"/>
+      <c r="K38" s="3"/>
+      <c r="L38" s="3"/>
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2"/>
+      <c r="I39" s="2"/>
+      <c r="J39" s="2"/>
+      <c r="K39" s="3"/>
+      <c r="L39" s="3"/>
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="3"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="3"/>
+      <c r="D40" s="3"/>
+      <c r="E40" s="3"/>
+      <c r="F40" s="3"/>
+      <c r="G40" s="3"/>
+      <c r="H40" s="3"/>
+      <c r="I40" s="3"/>
+      <c r="J40" s="3"/>
+      <c r="K40" s="3"/>
+      <c r="L40" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="7">
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
     <mergeCell ref="B4:C4"/>
     <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="B24:D24"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="C5:H20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D24" sqref="D24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="27.5703125" customWidth="1"/>
+    <col min="4" max="4" width="37.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.42578125" customWidth="1"/>
+    <col min="8" max="8" width="44" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C5" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="20" t="s">
+        <v>14</v>
+      </c>
+      <c r="G5" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="20" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="8" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C8" s="1">
+        <v>4</v>
+      </c>
+      <c r="D8" s="1">
+        <v>3</v>
+      </c>
+      <c r="G8" s="1">
+        <v>4</v>
+      </c>
+      <c r="H8" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C11" s="20" t="s">
+        <v>24</v>
+      </c>
+      <c r="D11" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H12" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C14" s="1">
+        <v>9</v>
+      </c>
+      <c r="D14" s="1">
+        <v>1</v>
+      </c>
+      <c r="G14" s="1">
+        <v>9</v>
+      </c>
+      <c r="H14" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="20" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C18" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C19" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+      <c r="C20" s="1">
+        <v>13</v>
+      </c>
+      <c r="D20" s="1">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="5">
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="C11:D11"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="C17:D17"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
EPBDS-7343 DT tables doesn't work with formulas. Fix DT tables with ranges.
--HG--
branch : 5.21.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7343_DT_with_formulas.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-7343_DT_with_formulas.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
-  <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <workbookPr defaultThemeVersion="124226" filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19440" windowHeight="11685" activeTab="1"/>
+    <workbookView windowHeight="11685" windowWidth="19440" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
-    <sheet name="DT" sheetId="13" r:id="rId1"/>
-    <sheet name="Tests" sheetId="14" r:id="rId2"/>
+    <sheet name="DT" r:id="rId1" sheetId="13"/>
+    <sheet name="Tests" r:id="rId2" sheetId="14"/>
   </sheets>
   <definedNames>
     <definedName name="_st1">#REF!</definedName>
@@ -26,7 +26,7 @@
     <author>Автор</author>
   </authors>
   <commentList>
-    <comment ref="B26" authorId="0" shapeId="0">
+    <comment authorId="0" ref="B26" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="52">
   <si>
     <t>Value</t>
   </si>
@@ -161,15 +161,70 @@
   <si>
     <t>Hour</t>
   </si>
+  <si>
+    <t>1.0;3.2</t>
+  </si>
+  <si>
+    <t>3.5;5.0</t>
+  </si>
+  <si>
+    <t>SimpleRules Double dt6(Double val)</t>
+  </si>
+  <si>
+    <t>Test dt6 dt6_Test</t>
+  </si>
+  <si>
+    <t>SimpleRules Double dt7(Double val)</t>
+  </si>
+  <si>
+    <t>=7</t>
+  </si>
+  <si>
+    <t>=new DoubleRange(1.0,3.2)</t>
+  </si>
+  <si>
+    <t>Test dt6 dt7_Test</t>
+  </si>
+  <si>
+    <t>Test dt7 dt7_Test</t>
+  </si>
+  <si>
+    <t>SimpleRules Double dt8(Double val)</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>7.0</t>
+  </si>
+  <si>
+    <t>SimpleRules Double dt8(Integer val)</t>
+  </si>
+  <si>
+    <t>=new IntgerRange(1,3)</t>
+  </si>
+  <si>
+    <t>4 .. 5</t>
+  </si>
+  <si>
+    <t>=new IntRange(1,3)</t>
+  </si>
+  <si>
+    <t>Test dt7 dt8_Test</t>
+  </si>
+  <si>
+    <t>Test dt8 dt8_Test</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="0"/>
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="000000" theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -267,7 +322,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.79998168889431442"/>
+        <fgColor rgb="1F497D" theme="3" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -296,7 +351,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -356,74 +411,92 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+  <cellStyleXfs count="2">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
   </cellStyleXfs>
-  <cellXfs count="21">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="24">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="1"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="2" fontId="5" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="3" fontId="5" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="4" fontId="6" numFmtId="0" quotePrefix="1" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="5" fontId="6" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="7" fontId="8" numFmtId="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="8" fontId="9" numFmtId="0" xfId="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="9" fontId="9" numFmtId="0" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="7" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="7" fontId="7" numFmtId="3" quotePrefix="1" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="10" fontId="7" numFmtId="0" quotePrefix="1" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="7" fontId="7" numFmtId="3" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="1" fillId="4" fontId="6" numFmtId="14" quotePrefix="1" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="7" fontId="8" numFmtId="0" xfId="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="2" fillId="6" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="3" fillId="6" fontId="4" numFmtId="0" xfId="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1" borderId="4" fillId="6" fontId="4" numFmtId="0" xfId="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf applyBorder="1" applyFill="1" applyFont="1" borderId="1" fillId="6" fontId="0" numFmtId="0" xfId="1"/>
+    <xf applyBorder="1" applyFont="1" borderId="5" fillId="0" fontId="0" numFmtId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="20% - Accent1 10" xfId="2"/>
-    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
-    <cellStyle name="Обычный 6" xfId="1"/>
+  <cellStyles count="2">
+    <cellStyle name="20% - Accent1 10" xfId="0"/>
+    <cellStyle builtinId="0" name="Обычный" xfId="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -440,10 +513,10 @@
   <a:themeElements>
     <a:clrScheme name="Стандартная">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="1F497D"/>
@@ -478,7 +551,7 @@
     </a:clrScheme>
     <a:fontScheme name="Стандартная">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -530,7 +603,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -635,7 +708,7 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="95000"/>
@@ -644,13 +717,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -660,7 +733,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="20000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -669,7 +742,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -678,7 +751,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw blurRad="40000" dir="5400000" dist="23000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -688,12 +761,12 @@
             <a:camera prst="orthographicFront">
               <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
+            <a:lightRig dir="t" rig="threePt">
               <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
+            <a:bevelT h="25400" w="63500"/>
           </a:sp3d>
         </a:effectStyle>
       </a:effectStyleLst>
@@ -724,7 +797,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+            <a:fillToRect b="180000" l="50000" r="50000" t="-80000"/>
           </a:path>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
@@ -743,7 +816,7 @@
             </a:gs>
           </a:gsLst>
           <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+            <a:fillToRect b="50000" l="50000" r="50000" t="50000"/>
           </a:path>
         </a:gradFill>
       </a:bgFillStyleLst>
@@ -755,21 +828,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:L40"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="A2:M61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F47" sqref="F47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="41.28515625" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="55.140625" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="19.28515625" customWidth="1"/>
-    <col min="6" max="6" width="42" customWidth="1"/>
-    <col min="7" max="7" width="65.42578125" customWidth="1"/>
-    <col min="8" max="8" width="31.85546875" customWidth="1"/>
+    <col min="2" max="2" customWidth="true" width="41.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="55.140625" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="42.0" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="65.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="31.85546875" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -802,18 +875,18 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="18" t="s">
         <v>13</v>
       </c>
-      <c r="C4" s="15" t="s">
+      <c r="C4" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="18" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="15" t="s">
+      <c r="G4" s="18" t="s">
         <v>7</v>
       </c>
       <c r="H4" s="2"/>
@@ -1046,18 +1119,18 @@
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="2"/>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="15" t="s">
+      <c r="C16" s="18" t="s">
         <v>7</v>
       </c>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="18" t="s">
         <v>20</v>
       </c>
-      <c r="G16" s="15" t="s">
+      <c r="G16" s="18" t="s">
         <v>7</v>
       </c>
       <c r="H16" s="2"/>
@@ -1206,14 +1279,18 @@
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="2"/>
-      <c r="B24" s="16" t="s">
+      <c r="B24" s="19" t="s">
         <v>31</v>
       </c>
-      <c r="C24" s="17"/>
-      <c r="D24" s="18"/>
+      <c r="C24" s="20"/>
+      <c r="D24" s="21"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="3"/>
-      <c r="G24" s="3"/>
+      <c r="F24" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>7</v>
+      </c>
       <c r="H24" s="3"/>
       <c r="I24" s="2"/>
       <c r="J24" s="2"/>
@@ -1222,16 +1299,20 @@
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="2"/>
-      <c r="B25" s="19" t="s">
+      <c r="B25" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="C25" s="19"/>
+      <c r="C25" s="17"/>
       <c r="D25" s="9" t="s">
         <v>3</v>
       </c>
       <c r="E25" s="2"/>
-      <c r="F25" s="3"/>
-      <c r="G25" s="3"/>
+      <c r="F25" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="H25" s="3"/>
       <c r="I25" s="2"/>
       <c r="J25" s="2"/>
@@ -1240,14 +1321,18 @@
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="2"/>
-      <c r="B26" s="19" t="s">
+      <c r="B26" s="17" t="s">
         <v>25</v>
       </c>
-      <c r="C26" s="19"/>
+      <c r="C26" s="17"/>
       <c r="D26" s="9"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
+      <c r="F26" s="15" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="8">
+        <v>1</v>
+      </c>
       <c r="H26" s="2"/>
       <c r="I26" s="2"/>
       <c r="J26" s="3"/>
@@ -1265,8 +1350,12 @@
         <v>30</v>
       </c>
       <c r="E27" s="2"/>
-      <c r="F27" s="3"/>
-      <c r="G27" s="3"/>
+      <c r="F27" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G27" s="8">
+        <v>2</v>
+      </c>
       <c r="H27" s="3"/>
       <c r="I27" s="2"/>
       <c r="J27" s="2"/>
@@ -1285,8 +1374,12 @@
         <v>1</v>
       </c>
       <c r="E28" s="2"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
+      <c r="F28" s="7">
+        <v>6</v>
+      </c>
+      <c r="G28" s="8">
+        <v>0</v>
+      </c>
       <c r="H28" s="3"/>
       <c r="I28" s="2"/>
       <c r="J28" s="2"/>
@@ -1305,8 +1398,12 @@
         <v>1</v>
       </c>
       <c r="E29" s="2"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
+      <c r="F29" s="7">
+        <v>7</v>
+      </c>
+      <c r="G29" s="8">
+        <v>3</v>
+      </c>
       <c r="H29" s="3"/>
       <c r="I29" s="2"/>
       <c r="J29" s="2"/>
@@ -1379,8 +1476,10 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
       <c r="E33" s="2"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="3"/>
+      <c r="F33" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="G33" s="18"/>
       <c r="H33" s="3"/>
       <c r="I33" s="2"/>
       <c r="J33" s="2"/>
@@ -1393,8 +1492,12 @@
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
       <c r="E34" s="2"/>
-      <c r="F34" s="2"/>
-      <c r="G34" s="2"/>
+      <c r="F34" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>1</v>
+      </c>
       <c r="H34" s="2"/>
       <c r="I34" s="2"/>
       <c r="J34" s="2"/>
@@ -1407,8 +1510,12 @@
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
       <c r="E35" s="2"/>
-      <c r="F35" s="2"/>
-      <c r="G35" s="2"/>
+      <c r="F35" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="G35" s="8">
+        <v>1</v>
+      </c>
       <c r="H35" s="2"/>
       <c r="I35" s="2"/>
       <c r="J35" s="2"/>
@@ -1421,8 +1528,12 @@
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
       <c r="E36" s="2"/>
-      <c r="F36" s="2"/>
-      <c r="G36" s="2"/>
+      <c r="F36" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="G36" s="8">
+        <v>2</v>
+      </c>
       <c r="H36" s="2"/>
       <c r="I36" s="2"/>
       <c r="J36" s="2"/>
@@ -1435,8 +1546,12 @@
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
       <c r="E37" s="2"/>
-      <c r="F37" s="2"/>
-      <c r="G37" s="2"/>
+      <c r="F37" s="7">
+        <v>6</v>
+      </c>
+      <c r="G37" s="8">
+        <v>0</v>
+      </c>
       <c r="H37" s="2"/>
       <c r="I37" s="2"/>
       <c r="J37" s="2"/>
@@ -1449,8 +1564,12 @@
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
       <c r="E38" s="2"/>
-      <c r="F38" s="2"/>
-      <c r="G38" s="2"/>
+      <c r="F38" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G38" s="8">
+        <v>3</v>
+      </c>
       <c r="H38" s="2"/>
       <c r="I38" s="2"/>
       <c r="J38" s="2"/>
@@ -1472,9 +1591,6 @@
       <c r="L39" s="3"/>
     </row>
     <row r="40" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A40" s="3"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
       <c r="D40" s="3"/>
       <c r="E40" s="3"/>
       <c r="F40" s="3"/>
@@ -1485,8 +1601,147 @@
       <c r="K40" s="3"/>
       <c r="L40" s="3"/>
     </row>
+    <row r="42">
+      <c r="B42" s="23" t="s">
+        <v>42</v>
+      </c>
+      <c r="C42" s="23"/>
+    </row>
+    <row r="43">
+      <c r="B43" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C43" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="B44" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C44" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="B45" s="16" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C45" s="16" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="B46" s="16" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C46" s="16" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="B47" s="16" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C47" s="16" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="B49" s="18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="18"/>
+    </row>
+    <row r="50">
+      <c r="B50" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="B51" s="15" t="s">
+        <v>49</v>
+      </c>
+      <c r="C51" s="8" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="B52" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C52" s="8" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="B53" s="7" t="n">
+        <v>6.0</v>
+      </c>
+      <c r="C53" s="8" t="n">
+        <v>0.0</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="B54" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="C54" s="8" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="B56" s="23" t="s">
+        <v>51</v>
+      </c>
+      <c r="C56" s="23"/>
+    </row>
+    <row r="57">
+      <c r="B57" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C57" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="B58" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C58" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="B59" s="16" t="n">
+        <v>3.0</v>
+      </c>
+      <c r="C59" s="16" t="n">
+        <v>1.0</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="B60" s="16" t="n">
+        <v>4.0</v>
+      </c>
+      <c r="C60" s="16" t="n">
+        <v>2.0</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="B61" s="16" t="n">
+        <v>7.0</v>
+      </c>
+      <c r="C61" s="16" t="n">
+        <v>3.0</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="F33:G33"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B4:C4"/>
@@ -1494,40 +1749,44 @@
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="F16:G16"/>
     <mergeCell ref="B24:D24"/>
+    <mergeCell ref="F24:G24"/>
+    <mergeCell ref="B42:C42"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="B56:C56"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup orientation="portrait" paperSize="9" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C5:H20"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B5:I27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="27.5703125" customWidth="1"/>
-    <col min="4" max="4" width="37.7109375" customWidth="1"/>
-    <col min="7" max="7" width="30.42578125" customWidth="1"/>
-    <col min="8" max="8" width="44" customWidth="1"/>
+    <col min="3" max="3" customWidth="true" width="27.5703125" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="37.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="44.0" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="5" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="D5" s="20" t="s">
+      <c r="D5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="G5" s="20" t="s">
+      <c r="G5" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="H5" s="20" t="s">
+      <c r="H5" s="22" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1574,16 +1833,16 @@
       </c>
     </row>
     <row r="11" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C11" s="20" t="s">
+      <c r="C11" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="D11" s="20" t="s">
+      <c r="D11" s="22" t="s">
         <v>15</v>
       </c>
-      <c r="G11" s="20" t="s">
+      <c r="G11" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="H11" s="20" t="s">
+      <c r="H11" s="22" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1629,15 +1888,15 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
-      <c r="C17" s="20" t="s">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C17" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="D17" s="20" t="s">
+      <c r="D17" s="22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="18" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C18" s="1" t="s">
         <v>25</v>
       </c>
@@ -1645,7 +1904,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C19" s="1" t="s">
         <v>33</v>
       </c>
@@ -1653,7 +1912,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C20" s="1">
         <v>13</v>
       </c>
@@ -1661,14 +1920,61 @@
         <v>2</v>
       </c>
     </row>
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B22" s="23" t="s">
+        <v>37</v>
+      </c>
+      <c r="C22" s="23"/>
+    </row>
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B23" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="C23" s="16" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="16" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="16">
+        <v>3</v>
+      </c>
+      <c r="C25" s="16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="16">
+        <v>4</v>
+      </c>
+      <c r="C26" s="16">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="16">
+        <v>7</v>
+      </c>
+      <c r="C27" s="16">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="6">
+    <mergeCell ref="B22:C22"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="C11:D11"/>
     <mergeCell ref="G11:H11"/>
     <mergeCell ref="C17:D17"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>